<commit_message>
finish reasoning step of start
</commit_message>
<xml_diff>
--- a/questions_with_reasoning.xlsx
+++ b/questions_with_reasoning.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>(a) ignore.</t>
+          <t xml:space="preserve"> The context of the sentence suggests that the sanctions were detrimental to the school's attempts at reform. The word "ignore" implies that the sanctions disregarded or overlooked the positive changes the school was trying to implement. The other options (b, c, d, e) do not fit as well because they do not convey the idea of negating or dismissing the school's efforts in the context of punitive measures. Thus, "ignore" accurately reflects the relationship between the sanctions and the school's efforts.</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>(b) populated areas.</t>
+          <t xml:space="preserve"> The phrase "where the people were" indicates that Sammy is looking for a location that is crowded or has a significant number of individuals. Among the options provided, "populated areas" (option b) is the most straightforward choice, as it directly refers to places where many people live or gather. While a race track may attract people during events, it is not consistently populated. The desert (option c) is sparsely inhabited, and an apartment (option d) may have few residents. A roadblock (option e) does not imply a gathering of people, but rather a stoppage. Therefore, option b is the best answer as it encompasses locations that are generally filled with people.</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(a) jewelry store.</t>
+          <t xml:space="preserve"> A choker is a type of necklace that is typically worn around the neck. If it is not found in a jewelry box or boutique, the most logical place to look for a choker would be a jewelry store, where a variety of jewelry items, including chokers, are available for purchase. The options 'b' (neck) and 'c' &amp; 'd' (jewelry box) do not represent places where one would typically seek to locate a choker for sale. 'e' (boutique) is also ruled out since the question specifies that we are looking for a choker not located in a boutique. Thus, option (a) is the only viable answer.</t>
         </is>
       </c>
     </row>
@@ -539,8 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>(d) atlas.
-Google Maps and other GPS services have replaced the need for physical atlases, which were once commonly used to navigate and plan routes. With the convenience and accuracy of digital maps on smartphones and other devices, physical atlases have become obsolete for many people. This shift in technology has made it easier for individuals to access up-to-date mapping information and navigate efficiently.</t>
+          <t xml:space="preserve"> Google Maps and similar GPS services provide digital navigation and mapping solutions that have largely replaced traditional paper atlases. Atlases are collections of maps that were commonly used for navigation before the advent of digital mapping technologies. With the convenience and real-time capabilities of GPS services, people now rely on these digital platforms for directions, traffic updates, and geographic information, making physical atlases largely obsolete for most users. The other options do not relate to navigation tools and do not fit the context of what has been replaced by digital maps.</t>
         </is>
       </c>
     </row>
@@ -562,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>(c) natural habitat. Foxes are wild animals that typically live in forests or other natural habitats. They are not known to look for pretty flowers, hen houses, storybooks, or dense forests specifically. The most logical choice is that the fox was looking for its natural habitat in the forest.</t>
+          <t xml:space="preserve"> The fox is a wild animal typically found in natural environments such as forests. When it walked from the city into the forest, it was likely seeking its natural habitat, which provides food, shelter, and space to roam. While options like "hen house" may seem plausible, they imply a domesticated setting which is not suitable for a fox. Additionally, "pretty flowers" and "storybook" are unrelated to a fox's needs, and "dense forest" describes the environment rather than something the fox is actively seeking. Therefore, the most logical answer is that the fox was looking for its natural habitat.</t>
         </is>
       </c>
     </row>
@@ -584,7 +583,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(d) television. Televisions typically require a cable connection to access cable television channels, which provide a variety of entertainment options. Radio shack, substation, cabinet, and desk are not typically associated with requiring a cable connection for home entertainment purposes.</t>
+          <t xml:space="preserve"> A television is a home entertainment device that typically requires cable to receive broadcast signals, whether through traditional cable systems or satellite services. While other options listed may involve electronic equipment or furniture, they do not serve as primary home entertainment devices that specifically rely on cable connections for functionality.</t>
         </is>
       </c>
     </row>
@@ -606,7 +605,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>(e) airport.</t>
+          <t xml:space="preserve"> The mention of a "drawstring bag" suggests that the woman is likely traveling, as such bags are commonly used for carrying personal items during trips. The context of checking baggage implies she is at a location where luggage is processed, which is typical at an airport. The other options do not logically fit with the act of checking a drawstring bag; for example, a garbage can, military, jewelry store, or safe do not require checked baggage in the same manner that air travel does. Therefore, the most reasonable destination for someone checking a drawstring bag is the airport.</t>
         </is>
       </c>
     </row>
@@ -628,7 +627,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>(b) refrigerator. The question mentions that the leftovers were covered in mold, which is a common occurrence when food is left for too long in a refrigerator where the temperature is conducive to mold growth. The other options such as carpet, breadbox, and coach are unlikely places for leftovers to be stored and therefore not the correct answer.</t>
+          <t xml:space="preserve"> The context of the question suggests that the forgotten leftovers are likely perishable food items, which would typically be stored in a cold environment to prevent spoilage. Among the options provided, both (b) refrigerator and (d) fridge refer to the same appliance used for storing food, but "refrigerator" is the more formal term. The other options, like (a) carpet, (c) breadbox, and (e) coach, are not suitable for storing leftovers as they do not provide the necessary conditions to keep food fresh. Therefore, the correct answer is (b) refrigerator, as it is the most logical place for someone to find old, moldy leftovers.</t>
         </is>
       </c>
     </row>
@@ -650,7 +649,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>(e) blotter.</t>
+          <t xml:space="preserve"> A blotter is specifically designed to absorb ink and prevent smudging when writing with a fountain pen or any ink-based writing instrument. It is typically made from absorbent paper that can soak up excess ink from the nib or from a freshly written line of text. The other options do not serve this purpose; for example, a shirt pocket or a calligrapher's hand would not effectively absorb ink, and an inkwell is used to hold ink rather than absorb it. A desk drawer does not relate to the absorption of ink at all. Thus, the correct choice is the blotter.</t>
         </is>
       </c>
     </row>
@@ -672,8 +671,1991 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>(d) business sector. 
-A business restaurant is likely to be located in a business sector because it caters to professionals and individuals working in that area. Business sectors are typically filled with offices, corporate buildings, and professionals who are looking for convenient dining options during their workday. Placing a business restaurant in a business sector increases the chances of attracting customers who are looking for a quick and efficient dining experience while on a break from work.</t>
+          <t xml:space="preserve"> A business restaurant is typically designed to cater to professionals and businesspeople who are looking for a convenient place to eat during work hours or business meetings. The business sector is characterized by offices, corporate buildings, and other workplaces where employees and clients are likely to gather for meals. This makes it an ideal location for a business restaurant, as it can attract a steady flow of customers who are looking for quick, professional dining options. In contrast, while locations like towns, hotels, and malls might have restaurants, they are not specifically tailored to serve the needs of business clientele in the same way that a restaurant situated in a business sector would be. Yellow pages, being a directory, do not represent a physical location.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Where do you put your grapes just before checking out?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>(a) mouth (b) grocery cart (c) super market (d) fruit basket (e) fruit market</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> When shopping for groceries, grapes are typically placed in a grocery cart while you continue to shop. Just before checking out, you would have already placed the grapes in the grocery cart along with other items. The other options do not accurately represent where you would put grapes in a grocery shopping context: (a) "mouth" is not a place for them while shopping, (c) "super market" refers to the location itself, not a storage option, (d) "fruit basket" implies a home storage solution rather than a shopping cart, and (e) "fruit market" indicates a type of store rather than a place to put grapes during the shopping process. Therefore, the correct answer is (b) grocery cart.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Before getting a divorce, what did the wife feel who was doing all the work?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>(a) harder (b) anguish (c) bitterness (d) tears (e) sadness</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The correct answer is "bitterness" because it reflects a deep-seated resentment and frustration that often arises when one partner feels overburdened and unappreciated in a relationship. In the context of a spouse doing all the work, bitterness can stem from feelings of inequality and a lack of acknowledgment for their contributions. While "anguish," "tears," and "sadness" also represent emotional pain, "bitterness" captures the specific sentiment of anger and resentment towards the situation and the other partner, making it the most fitting choice. "Harder" is not a suitable option as it does not convey an emotional state.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Johnny sat on a bench and relaxed after doing a lot of work on his hobby.  Where is he?</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>(a) state park (b) bus depot (c) garden (d) gym (e) rest area</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Johnny is described as sitting on a bench and relaxing, which suggests a calm and pleasant environment typically associated with leisure activities. Among the options, a garden is a place known for its tranquility and beauty, making it a suitable location for relaxation after engaging in a hobby. While a state park may also fit this description, a garden specifically emphasizes a serene and aesthetically pleasing setting. The other options, such as a bus depot, gym, and rest area, are not primarily associated with relaxation in the same way a garden is. Therefore, the most fitting answer is that Johnny is in a garden.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>James was cooling off two quickly.  He would die if he didn't find some way to stop what?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>(a) loss of heat (b) revenge (c) expansion (d) relaxation (e) calm down</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The phrase "cooling off too quickly" indicates that James is losing heat at a potentially dangerous rate. If he continues to lose heat excessively, it can lead to hypothermia or other life-threatening conditions. Therefore, the most logical answer is (a) loss of heat, as stopping the loss of heat is essential for his survival. The other options do not relate to a critical physical condition that could result in death.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Of all the rooms in a house it was his favorite, the aromas always drew him to the what?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>(a) yard (b) basement (c) kitchen (d) living room (e) garden</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The kitchen is typically associated with cooking and food preparation, which naturally involves various aromas from ingredients and meals being prepared. This connection to delightful smells makes the kitchen a favorite room for many people. The other options, such as the yard, basement, living room, and garden, do not evoke the same strong association with food-related aromas, making the kitchen the most logical answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Bill is stuck in marsh when a man comes up to him peaking Cajun, where is he?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>(a) low lands (b) new york (c) forest (d) louisiana (e) everglades</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The term "Cajun" specifically refers to a cultural group primarily found in Louisiana, known for their distinct French dialect and cultural heritage. The presence of a man speaking Cajun suggests that they are in a region where this culture is prevalent. Louisiana is famous for its marshlands, particularly in areas like the bayous, which aligns with Bill being stuck in a marsh. While "low lands" might be a general description, it does not pinpoint a specific location associated with Cajun culture. New York, forest, and everglades do not fit the context as closely as Louisiana does, making option (d) the correct answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>What is it called when you slowly cook using a grill?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>(a) backyard (b) restaurant (c) crockpot (d) neighbor's house (e) barbeque</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  
+The term "barbeque" specifically refers to a method of cooking where food, typically meat, is cooked slowly over indirect heat on a grill, often accompanied by smoke from wood or charcoal. This method enhances the flavor and tenderness of the food. The other options do not accurately describe this cooking technique: "backyard" refers to a location, "restaurant" refers to a place where food is served, "crockpot" is a slow-cooking appliance, and "neighbor's house" is simply a location where grilling could potentially occur but does not define the cooking method itself. Therefore, "barbeque" is the correct term for the process described in the question.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>What type of person typically contracts illness?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>(a) hospital (b) head (c) sick person (d) elderly person (e) doctor's office</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Elderly individuals are generally more susceptible to various illnesses due to a combination of factors, including a weakened immune system, the presence of chronic health conditions, and age-related physiological changes. These factors increase their vulnerability to infections and diseases compared to other demographics. While sick persons have already contracted an illness, the question specifically asks about who typically contracts illness, making the elderly person the most appropriate choice.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Where would you expect to find a pizzeria while shopping?</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>(a) chicago (b) street (c) little italy (d) food court (e) capital cities</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A food court is a designated area in a shopping complex or mall that features multiple food vendors, including pizzerias. It is specifically designed for dining while shopping, making it the most logical location to find a pizzeria among the options listed. While pizzerias can be found in cities like Chicago or areas known for Italian cuisine like Little Italy, the context of "while shopping" specifically points to a food court as a common place to find a variety of food options, including pizza, in close proximity to retail stores.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>When eating everything on the tasting menu, what does one tend to feel?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>(a) full stomach (b) getting full (c) gaining weight (d) sick (e) satisfaction</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> When experiencing a tasting menu, diners typically sample multiple small dishes rather than consuming a large quantity of food in one sitting. As a result, they may feel increasingly full as they progress through the menu, but not necessarily to the point of being overly stuffed or uncomfortable. The sensation of "getting full" captures the gradual feeling of fullness that accompanies enjoying a variety of flavors without overindulging, distinguishing it from the more definitive feeling of a "full stomach," which implies reaching the limit of one's capacity.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>What does playing soccer for a long time lead to?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>(a) excitement (b) fatigue (c) anger (d) hurting (e) getting tired</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Playing soccer for an extended period typically engages the body in vigorous physical activity, which can lead to physical exhaustion. "Getting tired" specifically captures the general experience of fatigue that accumulates over time during prolonged exercise. While option (b) "fatigue" is also related, "getting tired" is a more common and simpler expression that directly describes the sensation that comes from extended physical activity. The other options (a, c, d) are not direct outcomes of prolonged play and do not universally apply to the experience of playing soccer over time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Which entrance would you use if you do not want to use the back entrance?</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>(a) side (b) main (c) anterior (d) current (e) front</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The term "main entrance" typically refers to the primary or most prominent entry point of a building, which is often used by visitors. If a person is avoiding the back entrance, they are likely looking for the most accessible and commonly used entry, making the main entrance the most appropriate choice. Options like "side" or "front" could also be considered, but "main" clearly indicates the primary point of access. The terms "anterior" and "current" do not conventionally refer to entrances, further solidifying "main" as the correct answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>You can share files with someone if you have a connection to a what?</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>(a) freeway (b) radio (c) wires (d) computer network (e) electrical circuit</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A computer network is a system that connects computers and other devices together to share resources, such as files and data. While some of the other options involve connections (like radio or wires), they do not specifically pertain to the context of file sharing in a digital environment. A freeway, for instance, is unrelated to digital communications, and while electrical circuits can transmit signals, they do not inherently create a network for file sharing. Thus, a computer network is the most accurate answer for enabling file sharing.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>The accelerator was controller via a hand throttle, and the foot pedals controlled the steering in the small what?</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>(a) car (b) fuel system (c) accelerate (d) boat (e) airplane</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> In aviation, particularly in small aircraft, the accelerator is often controlled by a hand throttle rather than a foot pedal, which is more common in cars. The foot pedals in an airplane are typically used to control the rudder, which helps steer the aircraft. This configuration is distinct from cars, boats, and other options listed, making "airplane" the most fitting choice in this context.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Sean was lying about the body, but he was very scared.  He constantly worried about what?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>(a) the reward money (b) hurt feelings (c) being found out (d) problems (e) trouble</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sean's fear stems from the fact that he is lying about something significant and potentially incriminating (the body). In situations where someone is lying, especially about serious matters, the primary concern is often the fear of being discovered or exposed. This aligns with option (c) "being found out," as it directly relates to the consequences of his lie. While other options like (a) the reward money or (e) trouble might also be relevant, they do not capture the core anxiety of being exposed for dishonesty, which is the essence of Sean's fear in this scenario.</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>The drug kingpin told his man to run errands, this was code to go to all the dealers to do what they had?</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>(a) park (b) make time for (c) receive instructions (d) take money (e) leave work</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> In the context of drug trafficking, "running errands" typically involves collecting profits or payments from dealers. The phrase suggests that the man is being instructed to visit various dealers and ensure they are providing the expected financial returns to the kingpin. The option "take money" aligns with this interpretation, as it directly relates to the financial transactions that are central to the drug trade. The other options do not fit the context of the task at hand, making "take money" the most logical choice.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Though he could've kept going his body appreciated the rest, it had been constantly what during the day?</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>(a) walk (b) lay down (c) working (d) moving (e) exercise</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The phrase "constantly what during the day" implies an ongoing activity that requires physical effort. Among the options, "moving" best captures the idea of continuous physical activity without being too specific. "Working" (option c) could also imply effort but is less general than "moving". The other options (a, b, e) either suggest a more specific action (walking or exercising) or indicate rest (laying down), which does not fit with the context of the body needing rest from constant activity. Therefore, "moving" is the most appropriate choice as it encompasses a variety of physical activities that could lead to the need for rest.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Too many people want exotic snakes.  The demand is driving what to carry them?</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>(a) ditch (b) shop (c) north america (d) pet shops (e) outdoors</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The phrase "too many people want exotic snakes" indicates a growing interest and demand for these animals. This demand typically leads to businesses that cater to pet ownership, specifically those that sell pets and pet supplies. Among the options provided, "pet shops" (option d) are the most relevant as they are specifically designed to sell pets, including exotic snakes. Other options either do not pertain to the sale of pets (like 'ditch' or 'outdoors') or are too vague (like 'shop' or 'north america'). Therefore, the correct answer is that pet shops are the establishments that would be driven to carry exotic snakes due to the increasing demand.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Joe suffered many consequences from stabbing a stranger to death.   Among them, the family of the victim did something to him. What was that?</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>(a) knife wounds (b) buy a gun (c) bleeding (d) jail time (e) law suit</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> After the death of a loved one, it is common for families to seek legal recourse against the perpetrator. In this case, the family of the victim would likely file a lawsuit against Joe for wrongful death, seeking damages for their loss. The other options (a, b, c, d) do not directly involve actions taken by the victim's family in response to the crime. A law suit is a legal action initiated by the family, making it the correct answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>To prevent any glare during the big football game he made sure to clean the dust of his what?</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>(a) television (b) attic (c) corner (d) they cannot clean corner and library during football match they cannot need that (e) ground</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The question pertains to preventing glare during a football game, which suggests the need for a clear view of a screen where the game will be watched. The most logical option that aligns with this context is (a) television, as cleaning the dust off the TV would directly reduce glare and enhance visibility while watching the game. The other options, such as (b) attic and (c) corner, do not relate to viewing the game, and (d) does not provide a relevant action for the scenario. Option (e) ground could refer to the field where the game is played but is not related to the viewer's experience. Therefore, cleaning the television is the correct action to take.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>I have something in my head I want to share, what ways can I do that?</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>(a) write an essay (b) organize thoughts (c) speak information (d) summarize main points (e) have information</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> To share something that is in your head, one effective method is to "speak information." This option directly addresses the act of communicating thoughts verbally to others. While writing an essay (option a) or summarizing main points (option d) are also valid methods of sharing information, they involve a written format rather than an immediate verbal exchange. Organizing thoughts (option b) is a precursor to sharing but not a method of sharing in itself. Having information (option e) does not imply sharing; it simply indicates possession. Therefore, the most direct and relevant choice for sharing thoughts verbally is to "speak information."</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>He wanted a house that was gated off from other places, where should he start looking?</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>(a) neighborhood (b) subdivision (c) city (d) suburbs (e) street</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A subdivision typically refers to a residential area that has been divided into smaller plots of land, often featuring homes that share similar architectural styles and community amenities. Many subdivisions are designed to be gated communities, providing security and isolation from outside traffic and noise. In contrast, neighborhoods may or may not have gated options, cities are too broad and urban for gated residences, suburbs can include both gated and non-gated homes, and streets are too specific and limited in scope. Therefore, starting the search in a subdivision is the most logical choice for finding a gated house.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Where in Southern Europe would you find many canals?</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>(a) michigan (b) new york (c) amsterdam (d) venice (e) bridge</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Venice, located in Italy, is renowned for its extensive network of canals that serve as the primary mode of transportation within the city. The city's unique layout is characterized by waterways instead of roads, making it famous for its picturesque canals, gondolas, and bridges. Although Amsterdam is also known for its canals, it is located in Northern Europe, not Southern Europe. Therefore, the correct answer is Venice, as it is the prominent city associated with canals in Southern Europe.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>What would a camper need to do before he or she can start cooking food?</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>(a) make breakfast (b) go hiking (c) pack or bag (d) light fire (e) grab a match</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Before cooking food while camping, the camper must first establish a heat source, which is typically done by lighting a fire. This is essential for preparing most types of food, whether by direct cooking over the fire or using cookware placed on it. While options like grabbing a match (e) are related to starting a fire, they do not encompass the broader action of ensuring that the cooking process can begin by lighting the fire itself. Therefore, option (d) is the most comprehensive and necessary step for cooking food while camping.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>What could happen to a paper if you leave it outside even if it does not move?</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>(a) one material often recycled (b) ripped (c) saturated with water (d) one dimensional (e) crumpled</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> When paper is left outside, it is exposed to environmental elements such as rain, humidity, and moisture in the air. Even if the paper does not move, it can absorb water from these elements, leading to it becoming saturated. Saturation occurs when the paper absorbs more water than it can hold, resulting in a loss of structural integrity and making the paper soggy. Other options, such as being ripped or crumpled, could potentially occur as well, but saturation from water exposure is a direct and inevitable consequence of leaving paper outside in wet conditions.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Mark's semen was very thick, but after his vasectomy it was also what?</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>(a) blank (b) sparse (c) thin (d) clear (e) free flowing</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> After a vasectomy, the production of sperm is effectively halted as the vas deferens is cut or blocked, which can lead to changes in the consistency of the semen. The correct answer, "clear," indicates that the semen may lose its thickness and become more liquid or translucent in appearance, as it may no longer contain sperm, which can contribute to a thicker consistency. While "thin" might also seem plausible, "clear" is more accurate in describing the typical changes in the appearance of semen post-vasectomy.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>What is a great place to lay in the sun?</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>(a) in the basement (b) west (c) solar system (d) beach (e) beans</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The beach is a well-known and popular location for sunbathing due to its open exposure to sunlight, sandy areas, and the overall atmosphere conducive to relaxation and enjoyment of the sun. In contrast, the basement (a) is typically dark and does not receive sunlight, "west" (b) is a direction rather than a specific location, "solar system" (c) refers to a vast astronomical region rather than a place for sunbathing, and "beans" (e) is unrelated to sunbathing entirely. Therefore, the beach is the most appropriate and logical choice for laying in the sun.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Where would you find a seafood restaurant in the east coast of North America?</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>(a) maine (b) boston (c) beach town (d) coastal cities (e) ocean</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Maine is renowned for its seafood, particularly its lobsters and clams. The state has a rich maritime heritage and a strong fishing industry, making it a prime location for seafood restaurants. While Boston (option b) also has a variety of seafood options and coastal cities (option d) and beach towns (option c) may have seafood restaurants due to their proximity to the ocean, Maine is specifically famous for its seafood culture and is often considered a top destination for seafood enthusiasts. Therefore, option (a) is the most accurate answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>The president is the leader of what institution?</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>(a) walmart (b) white house (c) country (d) corporation (e) government</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The president serves as the head of state and government in a country, overseeing the executive branch and representing the nation domestically and internationally. While options (b) "White House" and (c) "country" are related, the term "government" encompasses the entire political system and structure that the president leads. Therefore, option (e) is the most accurate answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Sitting to close while watching TV can cause what sort of pain?</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>(a) brain problems (b) laziness (c) get fat (d) headache (e) laughter</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sitting too close to the TV can lead to eye strain due to the excessive effort required to focus on the screen. This strain can result in headaches, particularly if the viewer is exposed to bright lights or flickering images for extended periods. While other options may relate to lifestyle choices or effects of screen time, the direct consequence of sitting too close is primarily associated with discomfort in the eyes and subsequent headaches.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Where is a bald eagle safe?</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>(a) pine tree (b) open country (c) in washington (d) wildlife refuge (e) sky</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A wildlife refuge provides a protected environment where bald eagles can live without the threats posed by human activities, habitat destruction, and hunting. Wildlife refuges are specifically designed to preserve habitats for various species, including birds of prey like the bald eagle. While options like pine trees or the sky may offer temporary refuge, they do not provide the comprehensive protection and resources that a wildlife refuge does. Additionally, while Washington is home to many bald eagles, it does not guarantee safety compared to a designated wildlife refuge. Therefore, a wildlife refuge is the safest option for bald eagles.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>The game promised it was free, but the child's parents soon found themselves doing what for microtransactions?</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>(a) costly (b) captive (c) contained (d) paying (e) caught</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The phrase "found themselves doing what for microtransactions" implies that the parents were involved in a financial transaction related to the game. The term "paying" directly describes the action of exchanging money for in-game purchases, which aligns with the context of microtransactions. The other options, while they may convey a sense of being affected by the situation, do not specifically indicate a financial action. Therefore, "paying" is the most accurate and appropriate choice in this context.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>What kind of driving leads to accidents?</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>(a) stressful (b) dangerous (c) fun (d) illegal (e) deadly</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Dangerous driving refers to behaviors that significantly increase the risk of accidents, such as speeding, aggressive maneuvers, distracted driving, and driving under the influence of substances. While all the options can contribute to unsafe driving situations, "dangerous" specifically encapsulates the actions and conditions that directly lead to collisions and other traffic incidents. Stressful, fun, illegal, and deadly driving can all be associated with accidents, but "dangerous" most directly describes the nature of driving that results in increased accident rates.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>What is eating too much dinner likely to result in?</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>(a) tiredness (b) living longer (c) stomach ache (d) illness (e) acid reflux</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Eating too much dinner can lead to a feeling of fullness that exceeds the stomach's capacity, which often results in discomfort and pain in the abdominal area, commonly referred to as a stomach ache. This is due to the digestive system being overwhelmed by the excess food, which can cause bloating and cramping. While options like tiredness and acid reflux can also occur as a result of overeating, the most direct and immediate consequence of consuming too much food is typically a stomach ache. Therefore, option (c) is the most accurate answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>What is a person chatting with friends likely hoping to accomplish?</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>(a) gathering of information (b) communication (c) feel relaxed (d) kill boredom (e) social bonding</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> When a person chats with friends, they are primarily engaging in social bonding, which involves building and maintaining relationships. While other options such as communication (b) and feeling relaxed (c) may also be byproducts of the interaction, the core intent is often to strengthen connections and share experiences, which falls under social bonding (e). This interaction fosters a sense of belonging and community, making it the most fitting choice among the options provided.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Jame's bare feet were burned as he walked, because the sunshine had made the surface hot.  Where might he have been?</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>(a) disneyland (b) snow (c) windowsill (d) street (e) summer</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The question describes a scenario where James's bare feet were burned due to walking on a hot surface that had been heated by sunshine. Among the options provided, "street" (option d) is the most plausible location where the ground could become hot from direct sunlight, especially during warm weather. Streets are typically made of asphalt or concrete, materials that absorb and retain heat, making them uncomfortable to walk on with bare feet. The other options, such as (a) Disneyland, (b) snow, (c) windowsill, and (e) summer, do not directly imply a hot surface underfoot. While Disneyland could potentially have hot surfaces, it is too vague and does not specifically indicate the type of environment that could cause burns on bare feet. Snow would be cold, a windowsill doesn't typically represent a walking surface, and summer refers to a season rather than a specific location. Hence, option (d) "street" is the correct answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>A fox was thirsty searching for water during the drought, where was he?</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>(a) painting (b) hen house (c) california (d) virginia (e) movie hall</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The question describes a fox that is searching for water during a drought, which implies a dry environment where water sources are scarce. California is known for its significant drought conditions and water scarcity issues, making it a plausible location for a thirsty fox. The other options, such as a painting, hen house, and movie hall, do not represent realistic environments where a wild fox would naturally be found searching for water. Virginia, while it may experience droughts, is not as commonly associated with severe drought conditions as California. Therefore, California is the most logical answer based on the context provided.</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>What might be the result of a season of successful skiing?</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>(a) finish line (b) broken bones (c) broken legs (d) chapped lips (e) healthy body</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A season of successful skiing typically involves consistent practice and physical activity, which can lead to improved fitness levels, increased cardiovascular health, and enhanced muscle strength. Skiing is a full-body workout that engages various muscle groups and promotes overall health, making "healthy body" the most fitting result of successful skiing. The other options, while possible outcomes of skiing, do not reflect the positive results associated with a successful and enjoyable skiing season.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>The sensor would just the distance then set off an alarm, the installation expert explained it was called a what kind of sensor?</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>(a) near (b) closeness (c) here (d) proximity (e) this</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The term "proximity sensor" is commonly used in technology to describe a device that detects the presence or absence of an object within a certain range. These sensors are designed to measure the distance from the sensor to an object and can trigger an alarm or response when that object comes within a specified range. The other options, such as "near" and "closeness," do not accurately describe the type of sensor used in this context, as they are not standard terms used in the field of sensor technology. "Here" and "this" are also irrelevant in this context. Therefore, "proximity" is the correct and most appropriate choice.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>The man was eating lunch, but rushed when he looked at his watch, why did he rush?</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>(a) gain weight (b) late for work (c) heartburn (d) bad breath (e) early for work</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The context of the question indicates that the man was eating lunch and then suddenly rushed after checking his watch. This suggests that he became aware of time and realized he might not have enough left to finish his lunch before needing to go back to work or another commitment. Among the options provided, "late for work" (option b) is the most logical reason for his urgency, as it directly relates to needing to be on time for a responsibility. The other options do not adequately explain why he would rush while eating lunch.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>The evacuation became mandatory, so what came on the TV?</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>(a) advisory (b) mandate (c) soap opera (d) elective (e) optional</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> In the context of a mandatory evacuation, the information communicated on the TV would likely be an advisory that provides instructions, updates, and safety information to the public. An advisory is an official recommendation or warning, which is appropriate during emergencies. The other options either refer to non-emergency contexts (like a soap opera), or suggest voluntary actions (like elective or optional), which do not fit the urgency of a mandatory evacuation situation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>The person gave a good hands on what to show how to do the work?</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>(a) demonstration (b) garage (c) building (d) barn (e) synagogue</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The phrase "hands on" refers to a practical, direct approach to learning or showing how to do something. A "demonstration" is an example of this, as it involves showing someone how to perform a task or use a tool through practical application. The other options (garage, building, barn, synagogue) do not relate to the act of showing or teaching someone how to do work in a practical manner. Thus, option (a) is the best choice.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Where would you see some people doing jumping jacks?</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>(a) military base (b) opera (c) water fountain (d) bus stop (e) church</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Jumping jacks are a form of physical exercise commonly associated with fitness routines, warm-ups, or military training. A military base is a place where physical fitness is emphasized, and soldiers often engage in exercises like jumping jacks as part of their training. In contrast, the other options—an opera, water fountain, bus stop, and church—are not typically environments where people would perform such exercises.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>The body guard was good at his duties, he made the person who hired him what?</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>(a) better job (b) irritated (c) feel safe (d) save money (e) headache</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A bodyguard's primary responsibility is to provide protection and ensure the safety of the individual who has hired them. If the bodyguard is good at their duties, it implies that they are effectively safeguarding their client from potential threats or harm. This would naturally lead to the client feeling safe, as they can trust that their bodyguard is competently managing their security. The other options do not align with the role of a bodyguard; for example, 'irritated,' 'headache,' and 'better job' do not reflect the intended outcome of hiring a bodyguard, while 'save money' is not directly related to the function of providing safety. Therefore, the correct answer is (c) feel safe.</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Learning languages is difficult.  Even in a full immersion environment you're likely to make mistakes, mistakes will cause misinterpretation, which will be uncomfortable, which will cause what?,</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>(a) better communication (b) overthinking (c) frustration (d) misunderstandings (e) headaches</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> When learning a new language, making mistakes is a common experience, especially in an immersion setting where the pressure to communicate effectively is high. These mistakes can lead to misinterpretations of what is being said or intended, which can create uncomfortable social situations. This discomfort often results in frustration, as learners may feel inadequate or embarrassed about their language abilities. While options like "overthinking" and "misunderstandings" could also be seen as potential outcomes, the direct emotional response to the discomfort caused by misinterpretation is best captured by "frustration," making it the most fitting answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Jim enjoyed killing people, but he did it too often and the cops found out.  What might the cops do to him?</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>(a) going to jail (b) going to prison (c) beat him up (d) get arrested (e) die</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The most immediate action that law enforcement would take upon discovering that Jim has been killing people is to arrest him. "Getting arrested" refers to the process of being taken into custody by the police, which is the first step in the legal system following the discovery of a crime. While options (a) and (b) could be outcomes of the legal process after arrest, they do not reflect the initial action taken by the police. Options (c) and (e) are not lawful actions that police would take in response to a crime. Therefore, "get arrested" is the most appropriate and direct response to the situation described.</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Where is there usually a fiddle playing?</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>(a) music store (b) dance hall (c) orchestra (d) symphony (e) tennessee</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> In an orchestra, various string instruments, including the fiddle (which is often synonymous with the violin), are played. The environment of an orchestra is specifically designed for performing classical music, where the fiddle plays a significant role. While fiddles may also be played in dance halls (b) and other contexts, the term "orchestra" (c) is most directly associated with a formal setting where a fiddle is typically present and played as part of an ensemble. The other options do not specifically denote a setting where fiddles are regularly featured in a structured performance context.</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>What is the only was to recover from exhaustion?</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>(a) mediate (b) have rest (c) stay in bed (d) run out of steam (e) go to sleep</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Recovering from exhaustion fundamentally requires giving the body and mind a break. While options like "go to sleep" (e) can be part of recovery, it specifically implies a prolonged state of rest rather than simply taking a break. "Stay in bed" (c) may also suggest rest but does not encompass all forms of restorative activities. "Meditate" (a) could help alleviate mental fatigue but does not directly address physical exhaustion. "Run out of steam" (d) describes a state of exhaustion rather than a method of recovery. Therefore, the most comprehensive and direct answer that encompasses a general restorative activity is "have rest" (b), as it allows for a variety of restorative actions, whether it's sleeping, relaxing, or taking a break.</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>What would you do if you want to be able to earn money?</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>(a) apply for job (b) stand in line (c) take care of proposals (d) pass course (e) play the lottery</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Applying for a job is a direct and practical way to earn money, as it involves seeking employment where you can provide services or products in exchange for a salary or wages. The other options, while they may have indirect benefits or potential outcomes, do not directly lead to earning money. Standing in line does not generate income, taking care of proposals might be relevant in a specific context but does not guarantee earnings, passing a course could enhance job prospects but does not earn money by itself, and playing the lottery is a gamble with no guaranteed income. Therefore, applying for a job is the most effective action to take for earning money.</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>What is a grumpy person likely to have?</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>(a) headache (b) understand themselves (c) compliments (d) own house (e) happiness</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A grumpy person often exhibits irritability and discomfort, which can be linked to physical ailments such as headaches. Headaches can contribute to a person's grumpiness due to pain or discomfort, leading to a negative mood. In contrast, the other options—understanding themselves, receiving compliments, owning a house, or experiencing happiness—are less directly correlated with a grumpy disposition. A headache is a common reason for feeling irritable or grumpy, making it the most logical choice.</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>What do drugs do?</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>(a) damage (b) cloud mind (c) lower i.q (d) cause illness (e) cause accidents</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Drugs can impair judgment, coordination, and reaction times, leading to risky behaviors and potentially fatal accidents. While drugs can also cause damage, cloud the mind, lower IQ, and lead to illness, the most direct and immediate consequence of drug use in many cases is the increased likelihood of accidents, whether they be vehicular, workplace-related, or otherwise. Thus, option (e) reflects a critical and often highlighted risk associated with drug use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>A beaver can destroy a machines functionality if they build their dam in this?</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>(a) strip club (b) pocket (c) millpond (d) ontario (e) lake or river</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Beavers are known for building dams that can obstruct water flow and create ponds. A "millpond" is specifically a body of water that is created by damming a stream or river, often in conjunction with a mill. If a beaver builds a dam in a millpond, it can disrupt the water flow necessary for the machinery that operates in the mill, effectively destroying its functionality. While beavers can also impact lakes and rivers, the term "millpond" directly relates to machinery and its operation, making it the most relevant option.</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>They decided to hash things out over drinks, after enough booze they were able to get close on a few things and what?</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>(a) reach tentative agreement (b) suicide (c) examine thing (d) commit murder (e) stay in bed</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The phrase "hash things out" implies discussing and resolving issues or disagreements in a collaborative manner. In a context where individuals are drinking and attempting to come to a consensus, it is logical that after their discussions (enhanced by the effects of the drinks), they would be able to "reach a tentative agreement" on certain matters. The other options are either negative (such as suicide and murder) or unrelated to the context of resolving disputes, making (a) the most appropriate choice.</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Where could a fungus grow and not be disturbed by sunlight?</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>(a) under rocks (b) manhattan (c) toenails (d) grocery store (e) fallen tree</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fungi thrive in dark, humid environments where they are protected from sunlight, which can inhibit their growth and reproduction. Among the options given, "under rocks" provides a sheltered environment that would be consistently dark and damp, making it an ideal habitat for fungal growth. While "fallen tree" (option e) could also be a suitable environment for fungi due to the decaying wood providing nutrients, the question specifically asks for a location that is not disturbed by sunlight. Under rocks fits this criterion well, as it is typically covered and shielded from direct sunlight. The other options, such as "manhattan," "toenails," and "grocery store," either do not consistently provide the darkness needed for fungi or are not as ideal as the option of being under rocks.</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Can you name a good reason for attending school?</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>(a) get smart (b) boredom (c) colds and flu (d) taking tests (e) spend time</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  
+The primary purpose of attending school is to gain knowledge and develop critical thinking skills, which is encapsulated by the phrase "get smart." Education equips individuals with the intellectual tools necessary to understand the world, solve problems, and make informed decisions. While options (b) boredom), (c) colds and flu), (d) taking tests), and (e) spend time) may be associated with the school experience, they do not represent the fundamental purpose of education. Instead, they highlight negative or trivial aspects of schooling rather than the positive goal of intellectual growth and personal development that option (a) emphasizes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>What state south of Kentucky and north of Alabama will you find people playing the fiddle?</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>(a) alabama (b) tennessee (c) violin case (d) music store (e) bow and strings</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Tennessee is the state that lies directly south of Kentucky and north of Alabama. It is also known for its rich musical heritage, particularly in genres like country music, bluegrass, and folk, where the fiddle is commonly played. The other options do not represent states or relevant locations for this context. Therefore, Tennessee is the correct answer as it fits both the geographical and cultural criteria of the question.</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Though she made the cut years ago, its figurative scars would never what?</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>(a) joining (b) put together (c) stitch (d) heal (e) paste</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The phrase "figurative scars" suggests that the emotional or psychological impact of a past event is being referenced. In this context, "heal" is the most fitting choice because it implies the process of recovery from pain or trauma, which aligns with the idea of scars that represent lingering effects from the past. The other options (joining, put together, stitch, paste) do not convey the same sense of recovery or resolution, making "heal" the most appropriate answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>What does sex often make happen in people?</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>(a) making love (b) feel good (c) happyness (d) wonderful thing (e) cloud judgment</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  
+Sex often leads to the release of various hormones and neurotransmitters, such as oxytocin and endorphins, which are associated with feelings of pleasure and well-being. While options like "making love" (a) and "happyness" (c) could also be considered outcomes of sexual activity, they are more subjective or descriptive rather than direct physiological responses. "Wonderful thing" (d) is vague and does not specifically address the feeling associated with sex, and "cloud judgment" (e) implies a negative outcome that does not universally apply. Therefore, option (b) "feel good" is the most accurate answer, as it directly relates to the positive sensations that sex can produce in many individuals.</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Where would you see people in uniform playing with a ball?</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>(a) hole (b) television (c) sporting goods store (d) pool table (e) sporting event</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> People in uniform typically refers to athletes who represent a team, and they are most often seen playing in organized competitions known as sporting events. These events take place in various venues such as stadiums or arenas, where teams compete in games that usually involve a ball, such as football, basketball, or soccer. The other options do not represent a scenario where people in uniform play with a ball: a hole is ambiguous, television shows games but does not involve live play, a sporting goods store sells equipment but does not host games, and a pool table refers to a specific game rather than a team sport. Therefore, the most fitting answer is (e) sporting event.</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>What kind of place could have a seafood restaurant?</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>(a) new york (b) coastal cities (c) city (d) coastal cities (e) boston</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> While coastal cities (options b and d) are traditionally known for seafood restaurants due to their proximity to the ocean and access to fresh seafood, the term "city" (option c) is broader and encompasses various types of urban areas, including both coastal and non-coastal cities. Therefore, any city, regardless of its geographical location, could potentially have a seafood restaurant, making option c the most inclusive and correct answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Who was the head of the branch yelling at?</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>(a) owner (b) foot (c) subordinate (d) base (e) point</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The term "head of the branch" typically refers to a leader or manager within an organizational structure. In a workplace context, it is common for supervisors or managers to address, correct, or express frustration towards their subordinates, who are the employees that report directly to them. Therefore, the correct answer is (c) subordinate, as they are the most logical group that a head of a branch would be yelling at in the context of managing a team or department.</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>He made another call, he did this all day hoping people would what well to his offer?</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>(a) hang up (b) respond (c) contact (d) answer (e) attracting ducks</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The phrase "hoping people would respond well to his offer" implies that he is looking for a positive reaction from the individuals he is calling. The word "respond" suggests that he is expecting engagement or feedback regarding his offer. While "answer" (option d) could also relate to picking up the call, it does not convey the hope for a positive outcome as clearly as "respond." Therefore, option (b) is the most fitting choice in this context.</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>She needs to visit a bookshop after buying the latest fashion, where should she look?</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>(a) student union (b) mall (c) department store (d) library (e) town or city</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A mall typically houses a variety of retail shops, including bookshops and clothing stores. Given that she has already purchased the latest fashion, it is logical for her to look for a bookshop in the same location where she can find both clothing and books conveniently. While department stores may have limited book selections, they are not primarily focused on books like a dedicated bookshop in a mall would be. Other options, like a student union, library, or a general town or city, do not specifically suggest a place where both fashion and books are easily accessible together, making the mall the most suitable choice.</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Where could you see an advertisement while reading news?</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>(a) television (b) bus (c) email (d) web page (e) la ville</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  
+When reading news online, advertisements are commonly placed on web pages to attract the attention of readers. This is a standard practice in digital media where ads can be displayed alongside articles or in various formats such as banners, pop-ups, or sidebar ads. While advertisements can also be seen on television (a) and in emails (c), the context of "reading news" specifically pertains to online news platforms, making "web page" (d) the most relevant answer. Options like "bus" (b) and "la ville" (e) do not directly relate to reading news in the same context.</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>What is required to be good at playing tennis?</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>(a) tennis racket (b) skill (c) competition (d) tennis court (e) legs</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> To excel in playing tennis, the most essential requirement is skill. While having a tennis racket, access to a tennis court, and physical abilities such as strong legs are beneficial, they do not guarantee proficiency in the sport. Skill encompasses the ability to effectively hit the ball, understand game strategies, maintain consistency, and perform under pressure. Therefore, developing and honing skills is crucial for achieving success in tennis, making it the most fundamental requirement among the options provided.</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>What state is the John Davis  Lodge toll road found in?</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>(a) new jersey (b) eastern united states (c) good repair (d) connecticut (e) arizona</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The John Davis Lodge Toll Road, also known as Route 15, is located in Connecticut. This toll road connects several areas within the state and is named after John Davis Lodge, a former Governor of Connecticut. The other options do not accurately represent the location of the toll road, making (d) Connecticut the correct answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>The man went to clown college, he had always want to run away with the what?</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>(a) circus (b) carnival (c) surprise (d) spoons (e) party</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The phrase "run away with the circus" is a well-known expression that refers to leaving one's current life behind to join a traveling show, which typically includes clowns, acrobats, and other entertainers. Since the man attended clown college, it suggests that he aspires to be a clown, which is a common role within a circus. Therefore, the most fitting answer is (a) circus, as it directly relates to his aspirations and the context of clowning.</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Jamie wanted to reduce her waist size, but all of her efforts failed miserably.  She continued to do what?</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>(a) gain weight (b) augment (c) dispare (d) make larger (e) expand</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The context of the question indicates that Jamie was trying to reduce her waist size but was unsuccessful in her efforts. This implies that instead of achieving her goal of reduction, she experienced a change that is opposite to her intention. Among the options provided, "gain weight" (option a) is the only choice that aligns with the idea of her waist size not decreasing and suggests a negative outcome related to her weight loss attempts. The other options (augment, dispare, make larger, expand) either do not directly relate to gaining weight or are not appropriate in the context of waist size reduction. Thus, option (a) is the correct answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>James felt himself losing consciousness.  He was frightened.  He didn't want this.  He was scared of what?</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>(a) death (b) coma (c) peace (d) forgetfulness (e) loss of life</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> James's fear of losing consciousness indicates a concern about a serious and potentially fatal outcome. Among the options provided, "death" (a) encompasses the ultimate fear of no longer existing, which aligns with the context of feeling frightened in a situation where he might lose his awareness. While "coma" (b) and "loss of life" (e) are related to serious medical conditions and outcomes, they are not as direct as the fear of death itself. "Peace" (c) and "forgetfulness" (d) do not adequately capture the grave nature of his fear in this scenario. Therefore, the most logical and encompassing fear that James is experiencing is the fear of death.</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>If someone is aloof and self-important, what is their experience when meeting people?</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>(a) stress (b) nervousness (c) smile (d) being bored (e) making new friends</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> An aloof and self-important person typically exhibits a lack of interest in others and may feel superior to those they meet. This attitude can lead to a sense of boredom during social interactions, as they may not see value in engaging with people who do not meet their standards or expectations. Rather than feeling stressed or nervous, they are more likely to approach social situations with indifference, resulting in feelings of boredom.</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>He was receiving workman's compensation, he had tripped over a metal rod while building where?</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>(a) factory (b) construction site (c) engine (d) insides of skyscraper's walls (e) shops</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The phrase "tripped over a metal rod while building" suggests an environment where construction activities are taking place. Among the options provided, a "construction site" (option b) is the most fitting context for such an incident. Construction sites are places where various materials and equipment, including metal rods, are commonly present, making it plausible for someone to trip over them. The other options, such as factory or shops, may involve work-related injuries, but they do not specifically align with the context of "building" in the same way a construction site does. Therefore, option b is the correct answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>John and James spent most of their time communicating with each other on their project.  The time required to communicate slowed their what?</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>(a) static (b) train of thought. (c) progress (d) transfer of information (e) collaboration</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The question indicates that John and James spent a significant amount of time communicating, which implies that their communication was extensive and possibly inefficient. This prolonged communication likely detracted from the actual work they were doing on the project, leading to a slowdown in their overall progress. While options like "train of thought" and "collaboration" could also be affected, the most direct impact of spending too much time communicating is a decrease in the speed of completing their project, making "progress" the most appropriate choice.</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>When you play around with your dog they will have?</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>(a) alive (b) health (c) fun (d) playing dead (e) black</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> When you engage in play with your dog, the primary outcome is that both you and your dog experience enjoyment and pleasure from the interaction. The word "fun" directly captures the essence of what happens when you play together, as dogs are known for their playful nature and love for games. While options like "health" may be a secondary benefit of regular play, it does not directly address the immediate experience of playing. The other options, such as "alive," "playing dead," and "black," do not relate to the activities or feelings typically associated with playtime. Therefore, "fun" is the most appropriate answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Where would a person keep a book while it's being read?</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>(a) closet (b) library of congress (c) classroom (d) in bed (e) desk</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A desk is a common place where a person would keep a book while reading, as it provides a flat surface for the book to rest on and is often used for study or work purposes. While options like "in bed" (d) could also be a suitable place for reading, a desk is more associated with the act of studying or working with a book, making it the most logical choice among the options provided. The other options such as "closet" (a) and "library of congress" (b) are not practical for keeping a book while actively reading it, and "classroom" (c) does not imply personal ownership or ongoing use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>The student needed to  get some new pencils, where did he go?</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>(a) store (b) classroom (c) backpack (d) cabinet (e) teacher</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The student needed new pencils, which implies that he required a source for purchasing or acquiring them. Among the options provided, the "store" is the most logical place to obtain new pencils, as it is a location specifically designed for selling supplies. The other options, such as "classroom," "backpack," "cabinet," and "teacher," do not typically serve as primary sources for acquiring new pencils; they might contain existing supplies but wouldn't be associated with obtaining new ones. Therefore, the correct answer is (a) store.</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>She loved buying products, she was driven by her what to shop more than any practical needs?</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>(a) desire (b) money (c) time (d) credit (e) spending money</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The question asks for the underlying motivation that drives her to shop beyond practical needs. The term "desire" (option a) encapsulates the emotional and psychological urge to acquire products, regardless of necessity. While options like "money," "time," "credit," and "spending money" refer to resources or means that facilitate shopping, they do not represent the intrinsic motivation or passion for shopping itself. Desire signifies a strong feeling of wanting, which aligns perfectly with the context of shopping for pleasure rather than necessity.</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>How does getting paid feel?</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>(a) income tax (b) satisfaction (c) sorrow (d) ocean (e) bill collectors to happy</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Getting paid typically brings a sense of satisfaction because it represents the reward for effort and work completed. It signifies financial compensation for services rendered, which can lead to feelings of accomplishment and relief, especially if the payment meets financial needs. In contrast, options like "income tax" and "bill collectors" are associated with financial obligations or stress, while "sorrow" does not align with the positive experience of receiving payment. The term "ocean" is unrelated to the context of payment and feelings. Therefore, "satisfaction" is the most appropriate response to describe the feeling associated with getting paid.</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>The fat man refused to accept what was possible, he complained that he what the simplest activities?</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>(a) no go (b) unlikely (c) unable (d) cant do (e) impossibility</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The phrase "he complained that he" suggests that the man is expressing a sense of frustration or inability regarding his capacity to engage in activities. The option "can't do" (d) fits this context perfectly as it conveys a clear statement of inability. It aligns with the tone of complaint about the simplest activities and indicates a personal limitation. Other options like "no go," "unlikely," "unable," and "impossibility" do not fit the sentence structure as naturally or convey the same immediacy of frustration as "can't do."</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Where can meat last a long time?</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>(a) backery (b) ham sandwich (c) fridge (d) butcher shop (e) freezer</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The freezer is the best option for preserving meat for an extended period. Freezing slows down the growth of bacteria and other pathogens that cause food spoilage, allowing meat to be stored safely for several months or even years, depending on the type. While the fridge (option c) can also keep meat fresh, it typically only extends its shelf life for a few days to weeks. Options (a), (b), and (d) do not provide suitable long-term storage solutions for meat. Thus, the freezer is the optimal choice for longevity.</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>What group of musicians will include someone playing the cello?</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>(a) ocean (b) symphony (c) band (d) music store (e) music shop</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A symphony is an orchestral ensemble that typically includes a variety of string instruments, including the cello. The cello is a standard instrument in orchestras and symphonies, which focus on classical music performances. In contrast, a band generally features brass and woodwind instruments, while a music store or shop refers to a place to buy instruments rather than a group of musicians. The ocean is unrelated to music. Therefore, the most appropriate answer is "symphony."</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Where do bees congregate with red flowerS?</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>(a) trash can (b) honey (c) bouquet of flowers (d) rose garden (e) field of flowers</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Bees are attracted to flowers for their nectar and pollen, which are essential for their survival and the production of honey. Red flowers, such as those found in rose gardens, are particularly appealing to certain species of bees. While a bouquet of flowers (option c) may contain red flowers, it is a confined arrangement and not a natural habitat where bees typically congregate. A trash can (option a) is not related to flowers, and honey (option b) is a product made by bees, not a location. A field of flowers (option e) is a broader area where bees might also find red flowers, but the rose garden is specifically known for its abundant red blooms and is a more likely place for bees to gather. Therefore, the correct answer is (d) rose garden.</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>What is someone who gets angry after getting drunk likely to participate in?</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>(a) violence (b) falling down (c) vomiting (d) vomiting (e) lower standards</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> When individuals consume alcohol, it can impair their judgment and lower their inhibitions. For some, this can lead to aggressive behavior and increased irritability. If a person tends to become angry when intoxicated, they may be more likely to engage in violent actions as a response to conflicts or frustrations that arise while under the influence. Therefore, option (a) violence is the most appropriate choice, as it directly correlates with the behavior of getting angry after drinking. The other options, while potential effects of drinking, do not specifically relate to the angered state described in the question.</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>The teacher told all the students that listening was key, it was the main way they would gain what?</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>(a) empathy (b) anxiety (c) knowlege (d) falling down (e) hear things</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Listening is a fundamental skill that facilitates learning and understanding. When students actively listen, they absorb information, comprehend concepts, and enhance their overall knowledge base. The other options, such as empathy, anxiety, falling down, and hear things, do not directly relate to the primary educational goal of gaining knowledge through attentive listening. Therefore, option (c) knowledge is the most appropriate answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Stanley had a dream that was very vivid and scary. He had trouble telling it from what?</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>(a) reality (b) imagination (c) dreamworker (d) nightmare (e) awake</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The question describes a scenario where Stanley experiences a vivid and frightening dream, indicating that the dream was so intense that it blurred the lines between the dream state and real life. The phrase "had trouble telling it from" suggests a confusion between the experience of the dream and reality. While options like (b) imagination and (e) awake could also imply some level of confusion, the context of the dream being vivid and scary specifically points to reality as the primary point of confusion. Therefore, the best answer that fits this context is (a) reality.</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>The city's community garden was demolished for yet another what?</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>(a) wasteland (b) ocean (c) desert (d) parking lot (e) flowers</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The phrase "demolished for yet another" implies that the community garden was replaced by something that is often viewed as less beneficial or desirable. A parking lot is a common urban development that often leads to the destruction of green spaces, like community gardens, in favor of more concrete and utilitarian uses of land. In contrast, the other options do not logically fit; "wasteland," "ocean," and "desert" are not plausible replacements for a garden, and "flowers" would not be a reason for demolition. Therefore, "parking lot" is the most appropriate choice.</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>WHat do cats get into when they are ripping things apart?</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>(a) dog's mouth (b) floor (c) garage (d) trouble (e) nature</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> When cats engage in destructive behavior, such as ripping things apart, it often leads them to get into "trouble." This could mean getting scolded by their owners, damaging property, or even facing consequences from other pets in the household. The other options do not accurately reflect the situation—cats do not literally get into a dog's mouth, the floor is not a destination they get into, a garage is not specifically related to their behavior, and while "nature" could be an abstract idea, it doesn’t directly relate to the consequences of their actions. Thus, "trouble" is the most fitting and logical answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>What is a good result of losing weight?</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>(a) increased energy (b) healthier (c) loose skin (d) beauty (e) death</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Losing weight generally leads to improved health outcomes, such as lower risk of chronic diseases (like heart disease, diabetes, and hypertension), improved mobility, and better overall physical condition. While options like increased energy (a) can also be a benefit of weight loss, the most comprehensive and universally acknowledged positive result is becoming healthier (b). Loose skin (c) is often a side effect of significant weight loss, beauty (d) is subjective and varies from person to person, and death (e) is obviously a negative outcome. Therefore, the best choice indicating a good result of losing weight is (b) healthier.</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>A person lived in my what?</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>(a) demonstration (b) conference (c) building (d) garage (e) mouth</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The phrase "A person lived in my..." implies a physical space or shelter where someone resides. Out of the given options, "garage" (d) is the only one that typically refers to a space where a person might live or reside, even if it's unconventional. The other options do not represent living spaces: "demonstration" (a) and "conference" (b) are events, "building" (c) is a broader term that could include living spaces but is not specific enough, and "mouth" (e) is not a place where a person could live. Therefore, the most logical choice is (d) garage.</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>The skin was cut while chopping onions, where was this skin likely cut?</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>(a) good health (b) finger (c) meat (d) body (e) own family</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> When chopping onions, it is common for individuals to use a knife, which may lead to accidental cuts on their hands. The term "skin" in this context refers to the outer layer of the body, specifically on the fingers where such cuts are most likely to occur during food preparation. The other options do not relate directly to the act of chopping onions or the area where a person would typically get cut. Thus, "finger" is the most logical and accurate answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>What might you feel after doing housework for hours?</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>(a) anger (b) not boredom (c) stress (d) boredom (e) anxiety</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> After spending several hours doing housework, it's common to experience stress due to the physical exertion and the mental burden of completing chores. Housework can be demanding and time-consuming, leading to feelings of overwhelm or pressure to finish tasks. While other options like boredom or anxiety might also be possible, stress is a more direct and likely response to the prolonged effort and responsibility of housework.</t>
         </is>
       </c>
     </row>

</xml_diff>